<commit_message>
updates of 132kv transformer and cables
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6916DB-052E-435D-928D-06568A33010D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD991E71-0D10-4249-B2D2-05F40CA103FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26650" yWindow="-21390" windowWidth="16420" windowHeight="15300" tabRatio="500" firstSheet="198" activeTab="207" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="198" activeTab="207" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -21551,8 +21551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-C400-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -29825,7 +29825,7 @@
     <col min="12" max="1025" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="21" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
updated - cof in DKK
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD991E71-0D10-4249-B2D2-05F40CA103FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436ED969-F1FF-4C4A-AC61-A24006575053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="198" activeTab="207" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="81" activeTab="82" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -21551,7 +21551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-C400-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -29825,7 +29825,7 @@
     <col min="12" max="1025" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="21" t="s">
         <v>155</v>
       </c>
@@ -58060,8 +58060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
Found a mistake in table 233
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436ED969-F1FF-4C4A-AC61-A24006575053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BEBFA6-485A-4613-8EEE-4F9CA39C21DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="81" activeTab="82" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="233" activeTab="234" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -32454,8 +32454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DE00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -32502,7 +32502,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -32528,7 +32528,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="C3">
         <v>60</v>
@@ -32554,7 +32554,7 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -32580,7 +32580,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="C5">
         <v>60</v>
@@ -32606,7 +32606,7 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -32632,7 +32632,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -32658,7 +32658,7 @@
         <v>843</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C8">
         <v>25</v>
@@ -32684,7 +32684,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>25</v>
@@ -32710,7 +32710,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -58060,7 +58060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
found mistake in table 16
</commit_message>
<xml_diff>
--- a/data-raw/excel-spreadsheets/table_data.xlsx
+++ b/data-raw/excel-spreadsheets/table_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\CNAIM\data-raw\excel-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BEBFA6-485A-4613-8EEE-4F9CA39C21DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56D9A4A-7BEB-48B5-AA18-42DFA623DD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="233" activeTab="234" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="500" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -14381,8 +14381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -15581,7 +15581,7 @@
         <v>66</v>
       </c>
       <c r="B60" s="7">
-        <v>134796</v>
+        <v>87698</v>
       </c>
       <c r="C60" s="7">
         <v>23502</v>
@@ -15601,7 +15601,7 @@
         <v>67</v>
       </c>
       <c r="B61" s="7">
-        <v>263015</v>
+        <v>134796</v>
       </c>
       <c r="C61" s="7">
         <v>23502</v>
@@ -15621,7 +15621,7 @@
         <v>83</v>
       </c>
       <c r="B62" s="7">
-        <v>218932</v>
+        <v>263015</v>
       </c>
       <c r="C62" s="7">
         <v>36171</v>
@@ -32454,7 +32454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-DE00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>